<commit_message>
chore: rename and update files
Details
- Rename PCB_CAD.dwg to 亚克力夹层图纸.dwg
- Update 清单.xlsx with new content
- Update Claude settings

Impact
- User-facing: no
- Breaking change: no
</commit_message>
<xml_diff>
--- a/清单.xlsx
+++ b/清单.xlsx
@@ -251,31 +251,31 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -561,7 +561,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -573,327 +573,390 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <v>30</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5">
         <v>104</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
         <v>10</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
         <v>20</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5">
         <v>10</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5">
         <v>20</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
         <v>70</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
         <v>5</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>5</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
         <v>80</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
         <v>10</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5">
         <v>1</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
         <v>20</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
         <v>20</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
@@ -910,69 +973,6 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>